<commit_message>
fixed some errors in test descriptions
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/01a_AsTeRICS_Setup/Test_cases_AsTeRICS_installation_macosx.xlsx
+++ b/Tests/integrationTests/01a_AsTeRICS_Setup/Test_cases_AsTeRICS_installation_macosx.xlsx
@@ -146,9 +146,6 @@
     <t>Environment (OS + Version, Architecture, Java Version):</t>
   </si>
   <si>
-    <t>Install Asterics on Mac OSX (without embedded Java)</t>
-  </si>
-  <si>
     <t>ASTERICS_SETUP_MACOSX_1</t>
   </si>
   <si>
@@ -160,16 +157,20 @@
     <t>Test intallation of AsTeRICS on Mac OSX</t>
   </si>
   <si>
-    <t>asterics-are-xxx.tar.gz</t>
+    <t>Install Asterics on Mac OSX (with embedded Java)</t>
+  </si>
+  <si>
+    <t>asterics-are-javaembedded-xxx.dmg</t>
   </si>
   <si>
     <t>0. Deinstall AsTeRICS if already existing
-1. Extract asterics-are-xxx.tar.gz
-2. Install current Java 8  JRE (http://www.java.com/de/download/manual.jsp or through packet manager)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. ARE/start.sh must be executable and start without error message
-2. ARE/start_debug.sh must be executable and start without error message
+1. Install asterics-are-javaembedded-xxx.dmg by double clicking onto it.
+2. Search for 
+asterics-are
+in sportlight and start it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. ARE must start without error messages
 </t>
   </si>
 </sst>
@@ -549,7 +550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -560,7 +561,7 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="7" t="s">
@@ -594,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>10</v>
@@ -629,10 +630,10 @@
     </row>
     <row r="7" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>16</v>

</xml_diff>